<commit_message>
W miarę czysta wersja generowania xlsx dla Artificial intelligence
</commit_message>
<xml_diff>
--- a/xlsx/Artificial.xlsx
+++ b/xlsx/Artificial.xlsx
@@ -7,25 +7,40 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="AI" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Allianz SFIO Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>1M</t>
+  </si>
+  <si>
+    <t>2M</t>
+  </si>
+  <si>
+    <t>3M</t>
+  </si>
+  <si>
+    <t>6M</t>
+  </si>
+  <si>
+    <t>12M</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -85,7 +100,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -101,6 +116,24 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Wartość jednostki uczestnictwa</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -108,17 +141,28 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!B1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Allianz SFIO Artificial Intelligence</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>AI!A:A</c:f>
+              <c:f>Sheet1!A:A</c:f>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>AI!B:B</c:f>
+              <c:f>Sheet1!B:B</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="0"/>
@@ -174,6 +218,142 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Stopa zwrotu</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!B1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Allianz SFIO Artificial Intelligence</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:showVal val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$E$25:$I$25</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1M</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2M</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3M</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6M</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12M</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$26:$I$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-0.04300298129912361</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.0204364712409838</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0006612507084828856</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.01339328422462449</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.04787812840043526</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50020001"/>
+        <c:axId val="50020002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50020001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50020002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50020002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50020001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -184,10 +364,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -201,6 +381,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -494,13 +704,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:I86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -518,457 +728,703 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="3">
-        <v>43017</v>
+        <v>43015</v>
       </c>
       <c r="B3">
-        <v>105.7</v>
+        <v>105.71</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="3">
-        <v>43018</v>
+        <v>43016</v>
       </c>
       <c r="B4">
-        <v>106.79</v>
+        <v>105.71</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="3">
-        <v>43019</v>
+        <v>43017</v>
       </c>
       <c r="B5">
-        <v>106.9</v>
+        <v>105.7</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="3">
-        <v>43020</v>
+        <v>43018</v>
       </c>
       <c r="B6">
-        <v>107.35</v>
+        <v>106.79</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="3">
-        <v>43021</v>
+        <v>43019</v>
       </c>
       <c r="B7">
-        <v>107.34</v>
+        <v>106.9</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="3">
-        <v>43024</v>
+        <v>43020</v>
       </c>
       <c r="B8">
-        <v>107.2</v>
+        <v>107.35</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="3">
-        <v>43025</v>
+        <v>43021</v>
       </c>
       <c r="B9">
-        <v>107.18</v>
+        <v>107.34</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="3">
-        <v>43026</v>
+        <v>43022</v>
       </c>
       <c r="B10">
-        <v>106.96</v>
+        <v>107.34</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="3">
-        <v>43027</v>
+        <v>43023</v>
       </c>
       <c r="B11">
-        <v>107.09</v>
+        <v>107.34</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="3">
-        <v>43028</v>
+        <v>43024</v>
       </c>
       <c r="B12">
-        <v>106.68</v>
+        <v>107.2</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="3">
-        <v>43031</v>
+        <v>43025</v>
       </c>
       <c r="B13">
-        <v>107.24</v>
+        <v>107.18</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="3">
-        <v>43032</v>
+        <v>43026</v>
       </c>
       <c r="B14">
-        <v>106.84</v>
+        <v>106.96</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="3">
-        <v>43033</v>
+        <v>43027</v>
       </c>
       <c r="B15">
-        <v>106.96</v>
+        <v>107.09</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="3">
+        <v>43028</v>
+      </c>
+      <c r="B16">
+        <v>106.68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="3">
+        <v>43029</v>
+      </c>
+      <c r="B17">
+        <v>106.68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="3">
+        <v>43030</v>
+      </c>
+      <c r="B18">
+        <v>106.68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="3">
+        <v>43031</v>
+      </c>
+      <c r="B19">
+        <v>107.24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="3">
+        <v>43032</v>
+      </c>
+      <c r="B20">
+        <v>106.84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="3">
+        <v>43033</v>
+      </c>
+      <c r="B21">
+        <v>106.96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="3">
         <v>43034</v>
       </c>
-      <c r="B16">
+      <c r="B22">
         <v>105.98</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="3">
+    <row r="23" spans="1:9">
+      <c r="A23" s="3">
         <v>43035</v>
       </c>
-      <c r="B17">
+      <c r="B23">
         <v>107.14</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="3">
+    <row r="24" spans="1:9">
+      <c r="A24" s="3">
+        <v>43036</v>
+      </c>
+      <c r="B24">
+        <v>107.14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="3">
+        <v>43037</v>
+      </c>
+      <c r="B25">
+        <v>107.14</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" t="s">
+        <v>4</v>
+      </c>
+      <c r="I25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="3">
         <v>43038</v>
       </c>
-      <c r="B18">
+      <c r="B26">
         <v>108.14</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="3">
+      <c r="E26">
+        <v>-0.04300298129912361</v>
+      </c>
+      <c r="F26">
+        <v>-0.0204364712409838</v>
+      </c>
+      <c r="G26">
+        <v>0.0006612507084828856</v>
+      </c>
+      <c r="H26">
+        <v>0.01339328422462449</v>
+      </c>
+      <c r="I26">
+        <v>0.04787812840043526</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="3">
         <v>43039</v>
       </c>
-      <c r="B19">
+      <c r="B27">
         <v>108.55</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="3">
+    <row r="28" spans="1:9">
+      <c r="A28" s="3">
+        <v>43040</v>
+      </c>
+      <c r="B28">
+        <v>108.55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="3">
         <v>43041</v>
       </c>
-      <c r="B20">
+      <c r="B29">
         <v>108.97</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="3">
+    <row r="30" spans="1:9">
+      <c r="A30" s="3">
         <v>43042</v>
       </c>
-      <c r="B21">
+      <c r="B30">
         <v>108.26</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="3">
-        <v>43045</v>
-      </c>
-      <c r="B22">
-        <v>109.17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="3">
-        <v>43046</v>
-      </c>
-      <c r="B23">
-        <v>109.41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="3">
-        <v>43047</v>
-      </c>
-      <c r="B24">
-        <v>108.37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="3">
-        <v>43048</v>
-      </c>
-      <c r="B25">
-        <v>108.58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="3">
-        <v>43049</v>
-      </c>
-      <c r="B26">
-        <v>107.32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="3">
-        <v>43052</v>
-      </c>
-      <c r="B27">
-        <v>107.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="3">
-        <v>43053</v>
-      </c>
-      <c r="B28">
-        <v>107.66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="3">
-        <v>43054</v>
-      </c>
-      <c r="B29">
-        <v>107.33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="3">
-        <v>43055</v>
-      </c>
-      <c r="B30">
-        <v>106.86</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:9">
       <c r="A31" s="3">
-        <v>43056</v>
+        <v>43043</v>
       </c>
       <c r="B31">
-        <v>108.34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+        <v>108.26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" s="3">
-        <v>43059</v>
+        <v>43044</v>
       </c>
       <c r="B32">
-        <v>109.62</v>
+        <v>108.26</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="3">
-        <v>43060</v>
+        <v>43045</v>
       </c>
       <c r="B33">
-        <v>110.03</v>
+        <v>109.17</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="3">
-        <v>43061</v>
+        <v>43046</v>
       </c>
       <c r="B34">
-        <v>111.69</v>
+        <v>109.41</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="3">
-        <v>43062</v>
+        <v>43047</v>
       </c>
       <c r="B35">
-        <v>111.69</v>
+        <v>108.37</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="3">
-        <v>43063</v>
+        <v>43048</v>
       </c>
       <c r="B36">
-        <v>111.53</v>
+        <v>108.58</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="3">
-        <v>43066</v>
+        <v>43049</v>
       </c>
       <c r="B37">
-        <v>112.13</v>
+        <v>107.32</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="3">
-        <v>43067</v>
+        <v>43050</v>
       </c>
       <c r="B38">
-        <v>110.39</v>
+        <v>107.32</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="3">
-        <v>43068</v>
+        <v>43051</v>
       </c>
       <c r="B39">
-        <v>110.69</v>
+        <v>107.32</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="3">
-        <v>43069</v>
+        <v>43052</v>
       </c>
       <c r="B40">
-        <v>107.01</v>
+        <v>107.5</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="3">
-        <v>43070</v>
+        <v>43053</v>
       </c>
       <c r="B41">
-        <v>107.34</v>
+        <v>107.66</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="3">
-        <v>43073</v>
+        <v>43054</v>
       </c>
       <c r="B42">
-        <v>106.28</v>
+        <v>107.33</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="3">
-        <v>43074</v>
+        <v>43055</v>
       </c>
       <c r="B43">
-        <v>104.17</v>
+        <v>106.86</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="3">
-        <v>43075</v>
+        <v>43056</v>
       </c>
       <c r="B44">
-        <v>104.51</v>
+        <v>108.34</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="3">
-        <v>43076</v>
+        <v>43057</v>
       </c>
       <c r="B45">
-        <v>104.98</v>
+        <v>108.34</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="3">
-        <v>43077</v>
+        <v>43058</v>
       </c>
       <c r="B46">
-        <v>105.95</v>
+        <v>108.34</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="3">
-        <v>43080</v>
+        <v>43059</v>
       </c>
       <c r="B47">
-        <v>105.88</v>
+        <v>109.62</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="3">
-        <v>43081</v>
+        <v>43060</v>
       </c>
       <c r="B48">
-        <v>107.06</v>
+        <v>110.03</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="3">
-        <v>43082</v>
+        <v>43061</v>
       </c>
       <c r="B49">
-        <v>106.48</v>
+        <v>111.69</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="3">
-        <v>43083</v>
+        <v>43062</v>
       </c>
       <c r="B50">
-        <v>106.67</v>
+        <v>111.69</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="3">
-        <v>43084</v>
+        <v>43063</v>
       </c>
       <c r="B51">
-        <v>106.28</v>
+        <v>111.53</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="3">
-        <v>43087</v>
+        <v>43064</v>
       </c>
       <c r="B52">
-        <v>107.27</v>
+        <v>111.53</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="3">
-        <v>43088</v>
+        <v>43065</v>
       </c>
       <c r="B53">
-        <v>108.69</v>
+        <v>111.53</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="3">
-        <v>43089</v>
+        <v>43066</v>
       </c>
       <c r="B54">
-        <v>107.75</v>
+        <v>112.13</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="3">
-        <v>43090</v>
+        <v>43067</v>
       </c>
       <c r="B55">
-        <v>107.57</v>
+        <v>110.39</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="3">
-        <v>43091</v>
+        <v>43068</v>
       </c>
       <c r="B56">
-        <v>107.19</v>
+        <v>110.69</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="3">
-        <v>43096</v>
+        <v>43069</v>
       </c>
       <c r="B57">
-        <v>106.07</v>
+        <v>107.01</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="3">
-        <v>43097</v>
+        <v>43070</v>
       </c>
       <c r="B58">
-        <v>106.04</v>
+        <v>107.34</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="3">
+        <v>43071</v>
+      </c>
+      <c r="B59">
+        <v>107.34</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="3">
+        <v>43072</v>
+      </c>
+      <c r="B60">
+        <v>107.34</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="3">
+        <v>43073</v>
+      </c>
+      <c r="B61">
+        <v>106.28</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="3">
+        <v>43074</v>
+      </c>
+      <c r="B62">
+        <v>104.17</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="3">
+        <v>43075</v>
+      </c>
+      <c r="B63">
+        <v>104.51</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="3">
+        <v>43076</v>
+      </c>
+      <c r="B64">
+        <v>104.98</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="3">
+        <v>43077</v>
+      </c>
+      <c r="B65">
+        <v>105.95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="3">
+        <v>43078</v>
+      </c>
+      <c r="B66">
+        <v>105.95</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="3">
+        <v>43079</v>
+      </c>
+      <c r="B67">
+        <v>105.95</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="3">
+        <v>43080</v>
+      </c>
+      <c r="B68">
+        <v>105.88</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="3">
+        <v>43081</v>
+      </c>
+      <c r="B69">
+        <v>107.06</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="3">
+        <v>43082</v>
+      </c>
+      <c r="B70">
+        <v>106.48</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="3">
+        <v>43083</v>
+      </c>
+      <c r="B71">
+        <v>106.67</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="3">
+        <v>43084</v>
+      </c>
+      <c r="B72">
+        <v>106.28</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="3">
+        <v>43085</v>
+      </c>
+      <c r="B73">
+        <v>106.28</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="3">
+        <v>43086</v>
+      </c>
+      <c r="B74">
+        <v>106.28</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="3">
+        <v>43087</v>
+      </c>
+      <c r="B75">
+        <v>107.27</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="3">
+        <v>43088</v>
+      </c>
+      <c r="B76">
+        <v>108.69</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="3">
+        <v>43089</v>
+      </c>
+      <c r="B77">
+        <v>107.75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="3">
+        <v>43090</v>
+      </c>
+      <c r="B78">
+        <v>107.57</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="3">
+        <v>43091</v>
+      </c>
+      <c r="B79">
+        <v>107.19</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="3">
+        <v>43092</v>
+      </c>
+      <c r="B80">
+        <v>107.19</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="3">
+        <v>43093</v>
+      </c>
+      <c r="B81">
+        <v>107.19</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="3">
+        <v>43094</v>
+      </c>
+      <c r="B82">
+        <v>107.19</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="3">
+        <v>43095</v>
+      </c>
+      <c r="B83">
+        <v>107.19</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="3">
+        <v>43096</v>
+      </c>
+      <c r="B84">
+        <v>106.07</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="3">
+        <v>43097</v>
+      </c>
+      <c r="B85">
+        <v>106.04</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="3">
         <v>43098</v>
       </c>
-      <c r="B59">
+      <c r="B86">
         <v>105.93</v>
       </c>
     </row>

</xml_diff>

<commit_message>
generator ubrany w funkcję i powielony dla SFIO i SFIO
</commit_message>
<xml_diff>
--- a/xlsx/Artificial.xlsx
+++ b/xlsx/Artificial.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Artificial" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -145,7 +145,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!B1</c:f>
+              <c:f>Artificial!B1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -159,12 +159,12 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!A:A</c:f>
+              <c:f>Artificial!A:A</c:f>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!B:B</c:f>
+              <c:f>Artificial!B:B</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="0"/>
@@ -252,7 +252,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!B1</c:f>
+              <c:f>Artificial!B1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -266,7 +266,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$E$25:$I$25</c:f>
+              <c:f>Artificial!$E$25:$I$25</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -289,24 +289,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$26:$I$26</c:f>
+              <c:f>Artificial!$E$26:$I$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-0.04300298129912361</c:v>
+                  <c:v>0.05033011195100934</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.0204364712409838</c:v>
+                  <c:v>0.005496015388843034</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0006612507084828856</c:v>
+                  <c:v>0.03840696244442343</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.01339328422462449</c:v>
+                  <c:v>0.05022962112514362</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.04787812840043526</c:v>
+                  <c:v>0.07871462264150941</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -706,7 +706,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I86"/>
+  <dimension ref="A1:I93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -935,19 +935,19 @@
         <v>108.14</v>
       </c>
       <c r="E26" s="4">
-        <v>-0.04300298129912361</v>
+        <v>0.05033011195100934</v>
       </c>
       <c r="F26" s="4">
-        <v>-0.0204364712409838</v>
+        <v>0.005496015388843034</v>
       </c>
       <c r="G26" s="4">
-        <v>0.0006612507084828856</v>
+        <v>0.03840696244442343</v>
       </c>
       <c r="H26" s="4">
-        <v>0.01339328422462449</v>
+        <v>0.05022962112514362</v>
       </c>
       <c r="I26" s="4">
-        <v>0.04787812840043526</v>
+        <v>0.07871462264150941</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1428,6 +1428,62 @@
       </c>
       <c r="B86">
         <v>105.93</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="3">
+        <v>43099</v>
+      </c>
+      <c r="B87">
+        <v>105.93</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="3">
+        <v>43100</v>
+      </c>
+      <c r="B88">
+        <v>105.93</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="3">
+        <v>43101</v>
+      </c>
+      <c r="B89">
+        <v>105.93</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="3">
+        <v>43102</v>
+      </c>
+      <c r="B90">
+        <v>105.93</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="3">
+        <v>43103</v>
+      </c>
+      <c r="B91">
+        <v>107.65</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="3">
+        <v>43104</v>
+      </c>
+      <c r="B92">
+        <v>109.2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="3">
+        <v>43105</v>
+      </c>
+      <c r="B93">
+        <v>109.77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>